<commit_message>
parse Stuller Classic Bands Mens4
</commit_message>
<xml_diff>
--- a/Stuller Classic Bands Mens.xlsx
+++ b/Stuller Classic Bands Mens.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anne\Desktop\WEBSITE CONTENT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\J\canary.webremote.net\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15120" windowHeight="7965"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Stuller Classic Bands Mens" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="84">
   <si>
     <t>Model</t>
   </si>
@@ -116,129 +116,18 @@
     <t>18k Rose Gold</t>
   </si>
   <si>
-    <t>BHRL74M14W</t>
-  </si>
-  <si>
     <t>4mm</t>
   </si>
   <si>
-    <t>BHRL74M14Y</t>
-  </si>
-  <si>
-    <t>BHRL74M14R</t>
-  </si>
-  <si>
-    <t>BHRL74M18W</t>
-  </si>
-  <si>
-    <t>BHRL74M18Y</t>
-  </si>
-  <si>
-    <t>BHRL74MPT</t>
-  </si>
-  <si>
-    <t>BHRL74MPAL</t>
-  </si>
-  <si>
-    <t>BHRL75M14W</t>
-  </si>
-  <si>
-    <t>BHRL75M14Y</t>
-  </si>
-  <si>
-    <t>BHRL75M14R</t>
-  </si>
-  <si>
-    <t>BHRL75M18W</t>
-  </si>
-  <si>
-    <t>BHRL75M18Y</t>
-  </si>
-  <si>
-    <t>BHRL75M18R</t>
-  </si>
-  <si>
-    <t>BHRL75MPT</t>
-  </si>
-  <si>
-    <t>BHRL75MPAL</t>
-  </si>
-  <si>
     <t>5mm</t>
   </si>
   <si>
-    <t>BHRL76M14W</t>
-  </si>
-  <si>
-    <t>BHRL76M14Y</t>
-  </si>
-  <si>
-    <t>BHRL76M14R</t>
-  </si>
-  <si>
-    <t>BHRL76M18W</t>
-  </si>
-  <si>
-    <t>BHRL76M18Y</t>
-  </si>
-  <si>
-    <t>BHRL76M18R</t>
-  </si>
-  <si>
-    <t>BHRL76MPT</t>
-  </si>
-  <si>
-    <t>BHRL76MPAL</t>
-  </si>
-  <si>
     <t>6mm</t>
   </si>
   <si>
-    <t>BHRL77M14W</t>
-  </si>
-  <si>
-    <t>BHRL77M14Y</t>
-  </si>
-  <si>
-    <t>BHRL77M14R</t>
-  </si>
-  <si>
-    <t>BHRL77M18W</t>
-  </si>
-  <si>
-    <t>BHRL77M18Y</t>
-  </si>
-  <si>
-    <t>BHRL77MPT</t>
-  </si>
-  <si>
-    <t>BHRL77MPAL</t>
-  </si>
-  <si>
     <t>7mm</t>
   </si>
   <si>
-    <t>BHRL78M14W</t>
-  </si>
-  <si>
-    <t>BHRL78M14Y</t>
-  </si>
-  <si>
-    <t>BHRL78M14R</t>
-  </si>
-  <si>
-    <t>BHRL78M18W</t>
-  </si>
-  <si>
-    <t>BHRL78M18Y</t>
-  </si>
-  <si>
-    <t>BHRL78MPT</t>
-  </si>
-  <si>
-    <t>BHRL78MPAL</t>
-  </si>
-  <si>
     <t>8mm</t>
   </si>
   <si>
@@ -366,12 +255,33 @@
   </si>
   <si>
     <t xml:space="preserve">This classic 8mm wedding ring features a low profile and a lighter weight, providing excellent comfort for everyday wear. Crafted with pride in USA. </t>
+  </si>
+  <si>
+    <t>BHRL75M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Platinum </t>
+  </si>
+  <si>
+    <t>Palladium</t>
+  </si>
+  <si>
+    <t>BHRL74M</t>
+  </si>
+  <si>
+    <t>BHRL76M</t>
+  </si>
+  <si>
+    <t>BHRL77M</t>
+  </si>
+  <si>
+    <t>BHRL78M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -459,7 +369,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -773,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -855,28 +765,28 @@
     </row>
     <row r="2" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>20</v>
@@ -893,28 +803,28 @@
     </row>
     <row r="3" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>23</v>
@@ -931,28 +841,28 @@
     </row>
     <row r="4" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>24</v>
@@ -969,28 +879,28 @@
     </row>
     <row r="5" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>25</v>
@@ -1007,28 +917,28 @@
     </row>
     <row r="6" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>26</v>
@@ -1045,28 +955,28 @@
     </row>
     <row r="7" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>29</v>
@@ -1083,31 +993,31 @@
     </row>
     <row r="8" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>21</v>
@@ -1121,31 +1031,31 @@
     </row>
     <row r="9" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>21</v>
@@ -1159,28 +1069,28 @@
     </row>
     <row r="10" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>20</v>
@@ -1197,28 +1107,28 @@
     </row>
     <row r="11" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>23</v>
@@ -1235,28 +1145,28 @@
     </row>
     <row r="12" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>24</v>
@@ -1273,28 +1183,28 @@
     </row>
     <row r="13" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>25</v>
@@ -1311,28 +1221,28 @@
     </row>
     <row r="14" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>26</v>
@@ -1349,31 +1259,31 @@
     </row>
     <row r="15" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>21</v>
@@ -1387,31 +1297,31 @@
     </row>
     <row r="16" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>110</v>
+        <v>73</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>21</v>
@@ -1425,28 +1335,28 @@
     </row>
     <row r="17" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>88</v>
+        <v>51</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>20</v>
@@ -1463,28 +1373,28 @@
     </row>
     <row r="18" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>23</v>
@@ -1501,28 +1411,28 @@
     </row>
     <row r="19" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>24</v>
@@ -1539,28 +1449,28 @@
     </row>
     <row r="20" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>25</v>
@@ -1577,28 +1487,28 @@
     </row>
     <row r="21" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>92</v>
+        <v>55</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>92</v>
+        <v>55</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>26</v>
@@ -1615,28 +1525,28 @@
     </row>
     <row r="22" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>29</v>
@@ -1653,28 +1563,28 @@
     </row>
     <row r="23" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>94</v>
+        <v>57</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>94</v>
+        <v>57</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>27</v>
@@ -1691,28 +1601,28 @@
     </row>
     <row r="24" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>28</v>
@@ -1729,28 +1639,28 @@
     </row>
     <row r="25" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>20</v>
@@ -1767,28 +1677,28 @@
     </row>
     <row r="26" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>23</v>
@@ -1805,28 +1715,28 @@
     </row>
     <row r="27" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>24</v>
@@ -1843,28 +1753,28 @@
     </row>
     <row r="28" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>25</v>
@@ -1881,28 +1791,28 @@
     </row>
     <row r="29" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>26</v>
@@ -1919,28 +1829,28 @@
     </row>
     <row r="30" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>27</v>
@@ -1957,28 +1867,28 @@
     </row>
     <row r="31" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>28</v>
@@ -1995,28 +1905,28 @@
     </row>
     <row r="32" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>20</v>
@@ -2033,28 +1943,28 @@
     </row>
     <row r="33" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>104</v>
+        <v>67</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>104</v>
+        <v>67</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>23</v>
@@ -2071,28 +1981,28 @@
     </row>
     <row r="34" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>105</v>
+        <v>68</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>105</v>
+        <v>68</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>24</v>
@@ -2109,28 +2019,28 @@
     </row>
     <row r="35" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="J35" s="3" t="s">
         <v>25</v>
@@ -2147,28 +2057,28 @@
     </row>
     <row r="36" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="J36" s="3" t="s">
         <v>26</v>
@@ -2185,28 +2095,28 @@
     </row>
     <row r="37" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="J37" s="3" t="s">
         <v>27</v>
@@ -2223,28 +2133,28 @@
     </row>
     <row r="38" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="J38" s="3" t="s">
         <v>28</v>

</xml_diff>